<commit_message>
j'ai fait une modif en fait
si c'est vrai!
</commit_message>
<xml_diff>
--- a/cocuouccmoi.xlsx
+++ b/cocuouccmoi.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Coucou c'est moi</t>
+  </si>
+  <si>
+    <t>j'ai fait une modif!</t>
   </si>
 </sst>
 </file>
@@ -357,17 +360,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E6"/>
+  <dimension ref="C6:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>